<commit_message>
make sequelize use env variables
</commit_message>
<xml_diff>
--- a/public/excel/export.xlsx
+++ b/public/excel/export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -19,10 +19,604 @@
     <t>Email</t>
   </si>
   <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>ddd@d.com</t>
+    <t>User 1</t>
+  </si>
+  <si>
+    <t>user1@example.com</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>user2@example.com</t>
+  </si>
+  <si>
+    <t>User 3</t>
+  </si>
+  <si>
+    <t>user3@example.com</t>
+  </si>
+  <si>
+    <t>User 4</t>
+  </si>
+  <si>
+    <t>user4@example.com</t>
+  </si>
+  <si>
+    <t>User 5</t>
+  </si>
+  <si>
+    <t>user5@example.com</t>
+  </si>
+  <si>
+    <t>User 6</t>
+  </si>
+  <si>
+    <t>user6@example.com</t>
+  </si>
+  <si>
+    <t>User 7</t>
+  </si>
+  <si>
+    <t>user7@example.com</t>
+  </si>
+  <si>
+    <t>User 8</t>
+  </si>
+  <si>
+    <t>user8@example.com</t>
+  </si>
+  <si>
+    <t>User 9</t>
+  </si>
+  <si>
+    <t>user9@example.com</t>
+  </si>
+  <si>
+    <t>User 10</t>
+  </si>
+  <si>
+    <t>user10@example.com</t>
+  </si>
+  <si>
+    <t>User 11</t>
+  </si>
+  <si>
+    <t>user11@example.com</t>
+  </si>
+  <si>
+    <t>User 12</t>
+  </si>
+  <si>
+    <t>user12@example.com</t>
+  </si>
+  <si>
+    <t>User 13</t>
+  </si>
+  <si>
+    <t>user13@example.com</t>
+  </si>
+  <si>
+    <t>User 14</t>
+  </si>
+  <si>
+    <t>user14@example.com</t>
+  </si>
+  <si>
+    <t>User 15</t>
+  </si>
+  <si>
+    <t>user15@example.com</t>
+  </si>
+  <si>
+    <t>User 16</t>
+  </si>
+  <si>
+    <t>user16@example.com</t>
+  </si>
+  <si>
+    <t>User 17</t>
+  </si>
+  <si>
+    <t>user17@example.com</t>
+  </si>
+  <si>
+    <t>User 18</t>
+  </si>
+  <si>
+    <t>user18@example.com</t>
+  </si>
+  <si>
+    <t>User 19</t>
+  </si>
+  <si>
+    <t>user19@example.com</t>
+  </si>
+  <si>
+    <t>User 20</t>
+  </si>
+  <si>
+    <t>user20@example.com</t>
+  </si>
+  <si>
+    <t>User 21</t>
+  </si>
+  <si>
+    <t>user21@example.com</t>
+  </si>
+  <si>
+    <t>User 22</t>
+  </si>
+  <si>
+    <t>user22@example.com</t>
+  </si>
+  <si>
+    <t>User 23</t>
+  </si>
+  <si>
+    <t>user23@example.com</t>
+  </si>
+  <si>
+    <t>User 24</t>
+  </si>
+  <si>
+    <t>user24@example.com</t>
+  </si>
+  <si>
+    <t>User 25</t>
+  </si>
+  <si>
+    <t>user25@example.com</t>
+  </si>
+  <si>
+    <t>User 26</t>
+  </si>
+  <si>
+    <t>user26@example.com</t>
+  </si>
+  <si>
+    <t>User 27</t>
+  </si>
+  <si>
+    <t>user27@example.com</t>
+  </si>
+  <si>
+    <t>User 28</t>
+  </si>
+  <si>
+    <t>user28@example.com</t>
+  </si>
+  <si>
+    <t>User 29</t>
+  </si>
+  <si>
+    <t>user29@example.com</t>
+  </si>
+  <si>
+    <t>User 30</t>
+  </si>
+  <si>
+    <t>user30@example.com</t>
+  </si>
+  <si>
+    <t>User 31</t>
+  </si>
+  <si>
+    <t>user31@example.com</t>
+  </si>
+  <si>
+    <t>User 32</t>
+  </si>
+  <si>
+    <t>user32@example.com</t>
+  </si>
+  <si>
+    <t>User 33</t>
+  </si>
+  <si>
+    <t>user33@example.com</t>
+  </si>
+  <si>
+    <t>User 34</t>
+  </si>
+  <si>
+    <t>user34@example.com</t>
+  </si>
+  <si>
+    <t>User 35</t>
+  </si>
+  <si>
+    <t>user35@example.com</t>
+  </si>
+  <si>
+    <t>User 36</t>
+  </si>
+  <si>
+    <t>user36@example.com</t>
+  </si>
+  <si>
+    <t>User 37</t>
+  </si>
+  <si>
+    <t>user37@example.com</t>
+  </si>
+  <si>
+    <t>User 38</t>
+  </si>
+  <si>
+    <t>user38@example.com</t>
+  </si>
+  <si>
+    <t>User 39</t>
+  </si>
+  <si>
+    <t>user39@example.com</t>
+  </si>
+  <si>
+    <t>User 40</t>
+  </si>
+  <si>
+    <t>user40@example.com</t>
+  </si>
+  <si>
+    <t>User 41</t>
+  </si>
+  <si>
+    <t>user41@example.com</t>
+  </si>
+  <si>
+    <t>User 42</t>
+  </si>
+  <si>
+    <t>user42@example.com</t>
+  </si>
+  <si>
+    <t>User 43</t>
+  </si>
+  <si>
+    <t>user43@example.com</t>
+  </si>
+  <si>
+    <t>User 44</t>
+  </si>
+  <si>
+    <t>user44@example.com</t>
+  </si>
+  <si>
+    <t>User 45</t>
+  </si>
+  <si>
+    <t>user45@example.com</t>
+  </si>
+  <si>
+    <t>User 46</t>
+  </si>
+  <si>
+    <t>user46@example.com</t>
+  </si>
+  <si>
+    <t>User 47</t>
+  </si>
+  <si>
+    <t>user47@example.com</t>
+  </si>
+  <si>
+    <t>User 48</t>
+  </si>
+  <si>
+    <t>user48@example.com</t>
+  </si>
+  <si>
+    <t>User 49</t>
+  </si>
+  <si>
+    <t>user49@example.com</t>
+  </si>
+  <si>
+    <t>User 50</t>
+  </si>
+  <si>
+    <t>user50@example.com</t>
+  </si>
+  <si>
+    <t>User 51</t>
+  </si>
+  <si>
+    <t>user51@example.com</t>
+  </si>
+  <si>
+    <t>User 52</t>
+  </si>
+  <si>
+    <t>user52@example.com</t>
+  </si>
+  <si>
+    <t>User 53</t>
+  </si>
+  <si>
+    <t>user53@example.com</t>
+  </si>
+  <si>
+    <t>User 54</t>
+  </si>
+  <si>
+    <t>user54@example.com</t>
+  </si>
+  <si>
+    <t>User 55</t>
+  </si>
+  <si>
+    <t>user55@example.com</t>
+  </si>
+  <si>
+    <t>User 56</t>
+  </si>
+  <si>
+    <t>user56@example.com</t>
+  </si>
+  <si>
+    <t>User 57</t>
+  </si>
+  <si>
+    <t>user57@example.com</t>
+  </si>
+  <si>
+    <t>User 58</t>
+  </si>
+  <si>
+    <t>user58@example.com</t>
+  </si>
+  <si>
+    <t>User 59</t>
+  </si>
+  <si>
+    <t>user59@example.com</t>
+  </si>
+  <si>
+    <t>User 60</t>
+  </si>
+  <si>
+    <t>user60@example.com</t>
+  </si>
+  <si>
+    <t>User 61</t>
+  </si>
+  <si>
+    <t>user61@example.com</t>
+  </si>
+  <si>
+    <t>User 62</t>
+  </si>
+  <si>
+    <t>user62@example.com</t>
+  </si>
+  <si>
+    <t>User 63</t>
+  </si>
+  <si>
+    <t>user63@example.com</t>
+  </si>
+  <si>
+    <t>User 64</t>
+  </si>
+  <si>
+    <t>user64@example.com</t>
+  </si>
+  <si>
+    <t>User 65</t>
+  </si>
+  <si>
+    <t>user65@example.com</t>
+  </si>
+  <si>
+    <t>User 66</t>
+  </si>
+  <si>
+    <t>user66@example.com</t>
+  </si>
+  <si>
+    <t>User 67</t>
+  </si>
+  <si>
+    <t>user67@example.com</t>
+  </si>
+  <si>
+    <t>User 68</t>
+  </si>
+  <si>
+    <t>user68@example.com</t>
+  </si>
+  <si>
+    <t>User 69</t>
+  </si>
+  <si>
+    <t>user69@example.com</t>
+  </si>
+  <si>
+    <t>User 70</t>
+  </si>
+  <si>
+    <t>user70@example.com</t>
+  </si>
+  <si>
+    <t>User 71</t>
+  </si>
+  <si>
+    <t>user71@example.com</t>
+  </si>
+  <si>
+    <t>User 72</t>
+  </si>
+  <si>
+    <t>user72@example.com</t>
+  </si>
+  <si>
+    <t>User 73</t>
+  </si>
+  <si>
+    <t>user73@example.com</t>
+  </si>
+  <si>
+    <t>User 74</t>
+  </si>
+  <si>
+    <t>user74@example.com</t>
+  </si>
+  <si>
+    <t>User 75</t>
+  </si>
+  <si>
+    <t>user75@example.com</t>
+  </si>
+  <si>
+    <t>User 76</t>
+  </si>
+  <si>
+    <t>user76@example.com</t>
+  </si>
+  <si>
+    <t>User 77</t>
+  </si>
+  <si>
+    <t>user77@example.com</t>
+  </si>
+  <si>
+    <t>User 78</t>
+  </si>
+  <si>
+    <t>user78@example.com</t>
+  </si>
+  <si>
+    <t>User 79</t>
+  </si>
+  <si>
+    <t>user79@example.com</t>
+  </si>
+  <si>
+    <t>User 80</t>
+  </si>
+  <si>
+    <t>user80@example.com</t>
+  </si>
+  <si>
+    <t>User 81</t>
+  </si>
+  <si>
+    <t>user81@example.com</t>
+  </si>
+  <si>
+    <t>User 82</t>
+  </si>
+  <si>
+    <t>user82@example.com</t>
+  </si>
+  <si>
+    <t>User 83</t>
+  </si>
+  <si>
+    <t>user83@example.com</t>
+  </si>
+  <si>
+    <t>User 84</t>
+  </si>
+  <si>
+    <t>user84@example.com</t>
+  </si>
+  <si>
+    <t>User 85</t>
+  </si>
+  <si>
+    <t>user85@example.com</t>
+  </si>
+  <si>
+    <t>User 86</t>
+  </si>
+  <si>
+    <t>user86@example.com</t>
+  </si>
+  <si>
+    <t>User 87</t>
+  </si>
+  <si>
+    <t>user87@example.com</t>
+  </si>
+  <si>
+    <t>User 88</t>
+  </si>
+  <si>
+    <t>user88@example.com</t>
+  </si>
+  <si>
+    <t>User 89</t>
+  </si>
+  <si>
+    <t>user89@example.com</t>
+  </si>
+  <si>
+    <t>User 90</t>
+  </si>
+  <si>
+    <t>user90@example.com</t>
+  </si>
+  <si>
+    <t>User 91</t>
+  </si>
+  <si>
+    <t>user91@example.com</t>
+  </si>
+  <si>
+    <t>User 92</t>
+  </si>
+  <si>
+    <t>user92@example.com</t>
+  </si>
+  <si>
+    <t>User 93</t>
+  </si>
+  <si>
+    <t>user93@example.com</t>
+  </si>
+  <si>
+    <t>User 94</t>
+  </si>
+  <si>
+    <t>user94@example.com</t>
+  </si>
+  <si>
+    <t>User 95</t>
+  </si>
+  <si>
+    <t>user95@example.com</t>
+  </si>
+  <si>
+    <t>User 96</t>
+  </si>
+  <si>
+    <t>user96@example.com</t>
+  </si>
+  <si>
+    <t>User 97</t>
+  </si>
+  <si>
+    <t>user97@example.com</t>
+  </si>
+  <si>
+    <t>User 98</t>
+  </si>
+  <si>
+    <t>user98@example.com</t>
+  </si>
+  <si>
+    <t>User 99</t>
+  </si>
+  <si>
+    <t>user99@example.com</t>
+  </si>
+  <si>
+    <t>User 100</t>
+  </si>
+  <si>
+    <t>user100@example.com</t>
   </si>
 </sst>
 </file>
@@ -399,7 +993,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B101"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,6 +1012,798 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>